<commit_message>
initial commit to new dict
</commit_message>
<xml_diff>
--- a/data_processed/life_long_asthma.xlsx
+++ b/data_processed/life_long_asthma.xlsx
@@ -5,26 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smiie/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smiie/Desktop/RespiratoryHealth/data_processed/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BA99FA9-B4C7-1743-AF84-94C5A31B499E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{731C093D-8268-D446-A0F5-3D9C3BA4EF79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6640" yWindow="2060" windowWidth="24520" windowHeight="16120" xr2:uid="{843F71E1-CF07-8F41-B7F4-3AA7EBC774E6}"/>
+    <workbookView xWindow="3680" yWindow="2060" windowWidth="24520" windowHeight="16120" xr2:uid="{843F71E1-CF07-8F41-B7F4-3AA7EBC774E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$A$1</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$A$2:$A$22</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$B$1</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$B$2:$B$22</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$C$1</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$C$2:$C$22</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$D$1</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$D$2:$D$22</definedName>
-  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -54,10 +44,11 @@
     <t>Total Asthma in Thousands</t>
   </si>
   <si>
-    <t>Female</t>
+    <t>Male</t>
   </si>
   <si>
-    <t>Male</t>
+    <t>Female</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -65,7 +56,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="185" formatCode="0_);[Red]\(0\)"/>
+    <numFmt numFmtId="176" formatCode="0_);[Red]\(0\)"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -106,14 +97,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="185" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -432,8 +420,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50B5278D-23AE-8A49-A535-16B4B767538A}">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="O31" sqref="O31"/>
+    <sheetView tabSelected="1" zoomScale="107" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -451,17 +439,17 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2">
         <v>2021</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2">
         <v>41892</v>
       </c>
       <c r="C2" s="1">
@@ -475,7 +463,7 @@
       <c r="A3">
         <v>2020</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3">
         <v>42518</v>
       </c>
       <c r="C3" s="1">
@@ -489,7 +477,7 @@
       <c r="A4">
         <v>2019</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4">
         <v>41393</v>
       </c>
       <c r="C4" s="1">
@@ -503,7 +491,7 @@
       <c r="A5">
         <v>2018</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5">
         <v>41935</v>
       </c>
       <c r="C5" s="1">
@@ -517,7 +505,7 @@
       <c r="A6">
         <v>2017</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6">
         <v>42652</v>
       </c>
       <c r="C6" s="1">
@@ -531,7 +519,7 @@
       <c r="A7">
         <v>2016</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7">
         <v>43344</v>
       </c>
       <c r="C7" s="1">
@@ -545,7 +533,7 @@
       <c r="A8">
         <v>2015</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8">
         <v>40153</v>
       </c>
       <c r="C8" s="1">
@@ -559,7 +547,7 @@
       <c r="A9">
         <v>2014</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9">
         <v>40461</v>
       </c>
       <c r="C9" s="1">
@@ -573,7 +561,7 @@
       <c r="A10">
         <v>2013</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10">
         <v>37328</v>
       </c>
       <c r="C10" s="1">
@@ -587,7 +575,7 @@
       <c r="A11">
         <v>2012</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11">
         <v>39982</v>
       </c>
       <c r="C11" s="1">
@@ -601,7 +589,7 @@
       <c r="A12">
         <v>2011</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12">
         <v>39504</v>
       </c>
       <c r="C12" s="1">
@@ -615,7 +603,7 @@
       <c r="A13">
         <v>2010</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13">
         <v>39191</v>
       </c>
       <c r="C13" s="1">
@@ -629,7 +617,7 @@
       <c r="A14">
         <v>2009</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14">
         <v>39930</v>
       </c>
       <c r="C14" s="1">
@@ -643,7 +631,7 @@
       <c r="A15">
         <v>2008</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15">
         <v>38450</v>
       </c>
       <c r="C15" s="1">
@@ -657,7 +645,7 @@
       <c r="A16">
         <v>2007</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16">
         <v>34008</v>
       </c>
       <c r="C16" s="1">
@@ -671,7 +659,7 @@
       <c r="A17">
         <v>2006</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B17">
         <v>34132</v>
       </c>
       <c r="C17" s="1">
@@ -685,7 +673,7 @@
       <c r="A18">
         <v>2005</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18">
         <v>32621</v>
       </c>
       <c r="C18" s="1">
@@ -699,7 +687,7 @@
       <c r="A19">
         <v>2004</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B19">
         <v>30189</v>
       </c>
       <c r="C19" s="1">
@@ -713,7 +701,7 @@
       <c r="A20">
         <v>2003</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B20">
         <v>29768</v>
       </c>
       <c r="C20" s="1">
@@ -727,7 +715,7 @@
       <c r="A21">
         <v>2002</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B21">
         <v>30821</v>
       </c>
       <c r="C21" s="1">
@@ -741,7 +729,7 @@
       <c r="A22">
         <v>2001</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B22">
         <v>31354</v>
       </c>
       <c r="C22" s="1">

</xml_diff>